<commit_message>
fix: can remove css
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CohortsSimple.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CohortsSimple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE39518-443A-B344-8B18-D30C5B6C8DAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA9F06F-F737-8B45-B85D-72EAE1487C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="8" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -3137,9 +3137,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I82" sqref="I82"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3879,7 +3879,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J40" s="5" t="b">
         <v>1</v>
@@ -5062,7 +5062,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>546</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>546</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>546</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>546</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>546</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>546</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>546</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>546</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>546</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>546</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>546</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>546</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>546</v>
       </c>
@@ -5281,9 +5281,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5C5F0C-D2AD-1947-BA93-702C9678E896}">
   <dimension ref="A1:R140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q94" sqref="Q94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14357,7 +14357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE4DAAA-A03F-5441-93A5-04FBABBD777F}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>